<commit_message>
Reviewed Ivan input and added comments, made accurate changes to AdminUserStories
</commit_message>
<xml_diff>
--- a/AdminUserStories.xlsx
+++ b/AdminUserStories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Palej\Desktop\Software Design with AI for Cloud\Year_3\agile-labs3\Newsagent-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8033A192-083D-4601-9A43-863BDFFCEA75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB953594-E397-49DB-AF62-1A298E9631D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12130" yWindow="1190" windowWidth="23750" windowHeight="17800" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
+    <workbookView xWindow="19560" yWindow="1500" windowWidth="18290" windowHeight="17800" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="AdminUserStories" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="85">
   <si>
     <t>As an admin</t>
   </si>
@@ -285,6 +285,12 @@
   </si>
   <si>
     <t>Verify customerID is automatically assigned to new user</t>
+  </si>
+  <si>
+    <t>Verify message "customerID firstName/lastName was successfully created" is displayed</t>
+  </si>
+  <si>
+    <t>Verify customer doesn't already exist in database</t>
   </si>
 </sst>
 </file>
@@ -453,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -462,36 +468,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -502,97 +478,112 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -914,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB095BD-E922-497D-B7ED-398078A18E3D}">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:D19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -926,7 +917,7 @@
     <col min="2" max="2" width="13.08984375" customWidth="1"/>
     <col min="3" max="3" width="31.7265625" customWidth="1"/>
     <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="81" style="40" customWidth="1"/>
+    <col min="5" max="5" width="81" style="16" customWidth="1"/>
     <col min="6" max="6" width="63.7265625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -941,7 +932,7 @@
       <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="15" t="s">
         <v>63</v>
       </c>
       <c r="F1" s="5" t="s">
@@ -949,19 +940,19 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="14">
+      <c r="A2" s="30">
         <v>13</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="20" t="s">
         <v>51</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -969,11 +960,11 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="15"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="45" t="s">
+      <c r="A3" s="31"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="20" t="s">
         <v>69</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -981,703 +972,723 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="15"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="45" t="s">
+      <c r="A4" s="31"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="20" t="s">
         <v>71</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="15"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="45" t="s">
+      <c r="A5" s="31"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="20" t="s">
         <v>72</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="15"/>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="45" t="s">
+      <c r="A6" s="31"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="20" t="s">
         <v>56</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="15"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="45" t="s">
+      <c r="A7" s="31"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="20" t="s">
         <v>48</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="16"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
+      <c r="A9" s="30">
         <v>1</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="43" t="s">
+      <c r="E9" s="19" t="s">
         <v>57</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="7"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="44" t="s">
+      <c r="A10" s="31"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="20" t="s">
         <v>82</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="7"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="44" t="s">
+      <c r="A11" s="31"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="20" t="s">
         <v>65</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="7"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="44" t="s">
+      <c r="A12" s="31"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="20" t="s">
         <v>64</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="7"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="44" t="s">
+      <c r="A13" s="31"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="20" t="s">
         <v>66</v>
       </c>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="7"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="44" t="s">
+      <c r="A14" s="31"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="20" t="s">
         <v>67</v>
       </c>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="8"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="44" t="s">
+      <c r="A15" s="31"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="31"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="32"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="3"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="34"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="6">
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="3"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="30">
         <v>2</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B19" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C19" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D19" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="44" t="s">
+      <c r="E19" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="7"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="44" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="31"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="8"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="40" t="s">
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="32"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="3"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="34"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="6">
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="3"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="30">
         <v>3</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B23" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C23" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D23" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="44" t="s">
+      <c r="E23" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="7"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="44" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="31"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="8"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="44" t="s">
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="32"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="3"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="34"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="6">
-        <v>4</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="44" t="s">
-        <v>14</v>
-      </c>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="8"/>
+      <c r="A26" s="3"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
-      <c r="E26" s="44" t="s">
+      <c r="E26" s="21"/>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="30">
+        <v>4</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="32"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="3"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="34"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="6">
-        <v>5</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="8"/>
+      <c r="A29" s="3"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
-      <c r="E29" s="44" t="s">
+      <c r="E29" s="21"/>
+      <c r="F29" s="12"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="30">
+        <v>5</v>
+      </c>
+      <c r="B30" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="32"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F29" s="1"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="16"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-    </row>
-    <row r="31" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="20">
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="6"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+    </row>
+    <row r="33" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="38">
         <v>12</v>
       </c>
-      <c r="B31" s="21" t="s">
+      <c r="B33" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C33" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="21" t="s">
+      <c r="D33" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="47" t="s">
+      <c r="E33" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="F31" s="22"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" s="23"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="47" t="s">
+      <c r="F33" s="10"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="39"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="36"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="F32" s="22"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33" s="23"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="47" t="s">
+      <c r="F34" s="10"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="39"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F33" s="22"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="25"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="47" t="s">
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="40"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="37"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="F34" s="22"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="2"/>
-      <c r="B35" s="38"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="46"/>
-      <c r="F35" s="34"/>
-    </row>
-    <row r="36" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="20">
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="2"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="12"/>
+    </row>
+    <row r="38" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="38">
         <v>8</v>
       </c>
-      <c r="B36" s="21" t="s">
+      <c r="B38" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="C38" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="D36" s="21" t="s">
+      <c r="D38" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="E36" s="48" t="s">
+      <c r="E38" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F36" s="22"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="23"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="47" t="s">
+      <c r="F38" s="10"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="39"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F37" s="22"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A38" s="23"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="47" t="s">
+      <c r="F39" s="10"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="39"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F38" s="22"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="23"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="47" t="s">
+      <c r="F40" s="10"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="39"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="36"/>
+      <c r="E41" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F39" s="22"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="25"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="47" t="s">
+      <c r="F41" s="10"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="40"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="37"/>
+      <c r="E42" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="F40" s="22"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="3"/>
-      <c r="B41" s="37"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="37"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="34"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="20">
+      <c r="F42" s="10"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" s="3"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="12"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" s="38">
         <v>9</v>
       </c>
-      <c r="B42" s="21" t="s">
+      <c r="B44" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C42" s="21" t="s">
+      <c r="C44" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="D42" s="21" t="s">
+      <c r="D44" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E42" s="47" t="s">
+      <c r="E44" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="F42" s="22"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A43" s="23"/>
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="47" t="s">
+      <c r="F44" s="10"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" s="39"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="F43" s="22"/>
-    </row>
-    <row r="44" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A44" s="25"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="47" t="s">
+      <c r="F45" s="10"/>
+    </row>
+    <row r="46" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A46" s="40"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="F44" s="22"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="3"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="37"/>
-      <c r="D45" s="37"/>
-      <c r="E45" s="46"/>
-      <c r="F45" s="34"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A46" s="27">
+      <c r="F46" s="10"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" s="3"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="12"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" s="41">
         <v>10</v>
       </c>
-      <c r="B46" s="28" t="s">
+      <c r="B48" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="28" t="s">
+      <c r="C48" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="D46" s="28" t="s">
+      <c r="D48" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="E46" s="49" t="s">
+      <c r="E48" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="F46" s="50" t="s">
+      <c r="F48" s="25" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A47" s="30"/>
-      <c r="B47" s="31"/>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="49" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" s="42"/>
+      <c r="B49" s="45"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="F47" s="51"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" s="32"/>
-      <c r="B48" s="33"/>
-      <c r="C48" s="33"/>
-      <c r="D48" s="33"/>
-      <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" s="3"/>
-      <c r="B49" s="37"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="37"/>
-      <c r="E49" s="46"/>
-      <c r="F49" s="34"/>
+      <c r="F49" s="26"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="27">
+      <c r="A50" s="43"/>
+      <c r="B50" s="46"/>
+      <c r="C50" s="46"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51" s="3"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="12"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" s="41">
         <v>11</v>
       </c>
-      <c r="B50" s="28" t="s">
+      <c r="B52" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="C50" s="28" t="s">
+      <c r="C52" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="D50" s="28" t="s">
+      <c r="D52" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="E50" s="49" t="s">
+      <c r="E52" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="F50" s="29"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A51" s="30"/>
-      <c r="B51" s="31"/>
-      <c r="C51" s="31"/>
-      <c r="D51" s="31"/>
-      <c r="E51" s="49" t="s">
+      <c r="F52" s="11"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53" s="42"/>
+      <c r="B53" s="45"/>
+      <c r="C53" s="45"/>
+      <c r="D53" s="45"/>
+      <c r="E53" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="F51" s="29"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="32"/>
-      <c r="B52" s="33"/>
-      <c r="C52" s="33"/>
-      <c r="D52" s="33"/>
-      <c r="E52" s="49" t="s">
+      <c r="F53" s="11"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" s="43"/>
+      <c r="B54" s="46"/>
+      <c r="C54" s="46"/>
+      <c r="D54" s="46"/>
+      <c r="E54" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F52" s="29"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="38"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" s="9">
+      <c r="F54" s="11"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="14"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A58" s="33">
         <v>6</v>
       </c>
-      <c r="B56" s="9" t="s">
+      <c r="B58" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C56" s="9" t="s">
+      <c r="C58" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D56" s="9" t="s">
+      <c r="D58" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="E56" s="41" t="s">
+      <c r="E58" s="17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A57" s="10"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="41" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A59" s="34"/>
+      <c r="B59" s="34"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="34"/>
+      <c r="E59" s="17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="38"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A59" s="17">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="14"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61" s="7">
         <v>7</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="B61" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C59" s="17" t="s">
+      <c r="C61" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D59" s="17" t="s">
+      <c r="D61" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E59" s="42" t="s">
+      <c r="E61" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A60" s="18"/>
-      <c r="B60" s="18"/>
-      <c r="C60" s="18"/>
-      <c r="D60" s="18"/>
-      <c r="E60" s="42" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62" s="8"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A61" s="18"/>
-      <c r="B61" s="18"/>
-      <c r="C61" s="18"/>
-      <c r="D61" s="18"/>
-      <c r="E61" s="42" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A63" s="8"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="19"/>
-      <c r="B62" s="19"/>
-      <c r="C62" s="19"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="42" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A64" s="9"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="38"/>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A9:A15"/>
-    <mergeCell ref="B9:B15"/>
-    <mergeCell ref="C9:C15"/>
-    <mergeCell ref="D9:D15"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="D36:D40"/>
-    <mergeCell ref="C36:C40"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="C50:C52"/>
-    <mergeCell ref="D50:D52"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="D46:D48"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="C31:C34"/>
-    <mergeCell ref="D31:D34"/>
-    <mergeCell ref="A31:A34"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="B2:B7"/>
     <mergeCell ref="C2:C7"/>
     <mergeCell ref="D2:D7"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="C52:C54"/>
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="D48:D50"/>
+    <mergeCell ref="A9:A17"/>
+    <mergeCell ref="B9:B17"/>
+    <mergeCell ref="C9:C17"/>
+    <mergeCell ref="D9:D17"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="D38:D42"/>
+    <mergeCell ref="C38:C42"/>
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="B33:B36"/>
+    <mergeCell ref="C33:C36"/>
+    <mergeCell ref="D33:D36"/>
+    <mergeCell ref="A33:A36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Started on Planning Process and Architecture
</commit_message>
<xml_diff>
--- a/AdminUserStories.xlsx
+++ b/AdminUserStories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Palej\Desktop\Software Design with AI for Cloud\Year_3\agile-labs3\Newsagent-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB953594-E397-49DB-AF62-1A298E9631D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107BCD8E-CA22-4C0A-A6AB-3997B94F2FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19560" yWindow="1500" windowWidth="18290" windowHeight="17800" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
+    <workbookView xWindow="22890" yWindow="900" windowWidth="14030" windowHeight="19140" xr2:uid="{FDFDA4C7-506B-4F79-8102-C016FE887AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="AdminUserStories" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="88">
   <si>
     <t>As an admin</t>
   </si>
@@ -230,18 +230,6 @@
     <t>Acceptance criteria</t>
   </si>
   <si>
-    <t>Verify valid lastName &lt;= 15 characters</t>
-  </si>
-  <si>
-    <t>Verify valid firstName &lt;= 15 characters</t>
-  </si>
-  <si>
-    <t>Verify valid custAddress &lt;= 50 characters</t>
-  </si>
-  <si>
-    <t>Verify valid phoneNo &lt;= 9 digits followed by 0</t>
-  </si>
-  <si>
     <t>Valid userName example: admin</t>
   </si>
   <si>
@@ -291,6 +279,27 @@
   </si>
   <si>
     <t>Verify customer doesn't already exist in database</t>
+  </si>
+  <si>
+    <t>As a newsagent</t>
+  </si>
+  <si>
+    <t>Verify valid 0 &lt; firstName &lt;= 15 characters</t>
+  </si>
+  <si>
+    <t>Verify valid 0 &lt; lastName &lt;= 15 characters</t>
+  </si>
+  <si>
+    <t>Verify valid 0 &lt; custAddress &lt;= 50 characters</t>
+  </si>
+  <si>
+    <t>Phone number format 0 11 222 333 (total of 10 digits)</t>
+  </si>
+  <si>
+    <t>Verify valid phoneNo &lt;= 13 digits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Handle spaces on phoneNo and if cust enters +353 </t>
   </si>
 </sst>
 </file>
@@ -519,71 +528,71 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -907,18 +916,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB095BD-E922-497D-B7ED-398078A18E3D}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.90625" customWidth="1"/>
     <col min="2" max="2" width="13.08984375" customWidth="1"/>
-    <col min="3" max="3" width="31.7265625" customWidth="1"/>
+    <col min="3" max="3" width="28.453125" customWidth="1"/>
     <col min="4" max="4" width="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="81" style="16" customWidth="1"/>
-    <col min="6" max="6" width="63.7265625" customWidth="1"/>
+    <col min="5" max="5" width="74.36328125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="51.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -940,72 +949,72 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="30">
+      <c r="A2" s="28">
         <v>13</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="25" t="s">
         <v>50</v>
       </c>
       <c r="E2" s="20" t="s">
         <v>51</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="29"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="29"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="29"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="20" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="31"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="31"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="31"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="20" t="s">
-        <v>72</v>
-      </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="31"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
       <c r="E6" s="20" t="s">
         <v>56</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="31"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
       <c r="E7" s="20" t="s">
         <v>48</v>
       </c>
@@ -1020,98 +1029,102 @@
       <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="30">
+      <c r="A9" s="28">
         <v>1</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="25" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="31"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
       <c r="E10" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="29"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="31"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="20" t="s">
-        <v>65</v>
-      </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="31"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
       <c r="E12" s="20" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="31"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
       <c r="E13" s="20" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="31"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
+    <row r="14" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="29"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
       <c r="E14" s="20" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="31"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
+    <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="29"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
       <c r="E15" s="20" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="31"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
       <c r="E16" s="20" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="32"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
       <c r="E17" s="20" t="s">
         <v>16</v>
       </c>
@@ -1126,42 +1139,42 @@
       <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="30">
+      <c r="A19" s="28">
         <v>2</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="27" t="s">
+      <c r="D19" s="25" t="s">
         <v>7</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>45</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="31"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
       <c r="E20" s="20" t="s">
         <v>46</v>
       </c>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="32"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
+      <c r="A21" s="30"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
       <c r="E21" s="16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F21" s="1"/>
     </row>
@@ -1174,40 +1187,40 @@
       <c r="F22" s="12"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="30">
+      <c r="A23" s="28">
         <v>3</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D23" s="27" t="s">
+      <c r="D23" s="25" t="s">
         <v>10</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>14</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="31"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
+      <c r="A24" s="29"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
       <c r="E24" s="20" t="s">
         <v>39</v>
       </c>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="32"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
+      <c r="A25" s="30"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
       <c r="E25" s="20" t="s">
         <v>11</v>
       </c>
@@ -1222,16 +1235,16 @@
       <c r="F26" s="12"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" s="30">
+      <c r="A27" s="28">
         <v>4</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="25" t="s">
         <v>12</v>
       </c>
       <c r="E27" s="20" t="s">
@@ -1240,10 +1253,10 @@
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" s="32"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
       <c r="E28" s="20" t="s">
         <v>15</v>
       </c>
@@ -1258,30 +1271,30 @@
       <c r="F29" s="12"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="30">
+      <c r="A30" s="28">
         <v>5</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="27" t="s">
+      <c r="D30" s="25" t="s">
         <v>18</v>
       </c>
       <c r="E30" s="20" t="s">
         <v>19</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="32"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
+      <c r="A31" s="30"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
       <c r="E31" s="20" t="s">
         <v>20</v>
       </c>
@@ -1296,16 +1309,16 @@
       <c r="F32" s="12"/>
     </row>
     <row r="33" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="38">
+      <c r="A33" s="34">
         <v>12</v>
       </c>
-      <c r="B33" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" s="35" t="s">
+      <c r="B33" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="35" t="s">
+      <c r="D33" s="31" t="s">
         <v>54</v>
       </c>
       <c r="E33" s="22" t="s">
@@ -1314,30 +1327,30 @@
       <c r="F33" s="10"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="39"/>
-      <c r="B34" s="36"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
+      <c r="A34" s="35"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
       <c r="E34" s="22" t="s">
         <v>52</v>
       </c>
       <c r="F34" s="10"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="39"/>
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
+      <c r="A35" s="35"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
       <c r="E35" s="22" t="s">
         <v>47</v>
       </c>
       <c r="F35" s="10"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A36" s="40"/>
-      <c r="B36" s="37"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="37"/>
+      <c r="A36" s="36"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
       <c r="E36" s="22" t="s">
         <v>48</v>
       </c>
@@ -1352,16 +1365,16 @@
       <c r="F37" s="12"/>
     </row>
     <row r="38" spans="1:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="38">
+      <c r="A38" s="34">
         <v>8</v>
       </c>
-      <c r="B38" s="35" t="s">
-        <v>59</v>
-      </c>
-      <c r="C38" s="35" t="s">
+      <c r="B38" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="D38" s="35" t="s">
+      <c r="D38" s="31" t="s">
         <v>61</v>
       </c>
       <c r="E38" s="23" t="s">
@@ -1370,40 +1383,40 @@
       <c r="F38" s="10"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="39"/>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
       <c r="E39" s="22" t="s">
         <v>27</v>
       </c>
       <c r="F39" s="10"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A40" s="39"/>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
+      <c r="A40" s="35"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
       <c r="E40" s="22" t="s">
         <v>28</v>
       </c>
       <c r="F40" s="10"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A41" s="39"/>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
+      <c r="A41" s="35"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
       <c r="E41" s="22" t="s">
         <v>29</v>
       </c>
       <c r="F41" s="10"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A42" s="40"/>
-      <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="37"/>
+      <c r="A42" s="36"/>
+      <c r="B42" s="33"/>
+      <c r="C42" s="33"/>
+      <c r="D42" s="33"/>
       <c r="E42" s="22" t="s">
         <v>25</v>
       </c>
@@ -1418,16 +1431,16 @@
       <c r="F43" s="12"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A44" s="38">
+      <c r="A44" s="34">
         <v>9</v>
       </c>
-      <c r="B44" s="35" t="s">
+      <c r="B44" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="C44" s="35" t="s">
+      <c r="C44" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="D44" s="35" t="s">
+      <c r="D44" s="31" t="s">
         <v>31</v>
       </c>
       <c r="E44" s="22" t="s">
@@ -1436,20 +1449,20 @@
       <c r="F44" s="10"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A45" s="39"/>
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
       <c r="E45" s="22" t="s">
         <v>43</v>
       </c>
       <c r="F45" s="10"/>
     </row>
     <row r="46" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A46" s="40"/>
-      <c r="B46" s="37"/>
-      <c r="C46" s="37"/>
-      <c r="D46" s="37"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="33"/>
+      <c r="C46" s="33"/>
+      <c r="D46" s="33"/>
       <c r="E46" s="22" t="s">
         <v>44</v>
       </c>
@@ -1464,40 +1477,40 @@
       <c r="F47" s="12"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A48" s="41">
+      <c r="A48" s="39">
         <v>10</v>
       </c>
-      <c r="B48" s="44" t="s">
+      <c r="B48" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="C48" s="44" t="s">
+      <c r="C48" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="D48" s="44" t="s">
+      <c r="D48" s="42" t="s">
         <v>41</v>
       </c>
       <c r="E48" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="F48" s="25" t="s">
-        <v>80</v>
+      <c r="F48" s="37" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" s="42"/>
-      <c r="B49" s="45"/>
-      <c r="C49" s="45"/>
-      <c r="D49" s="45"/>
+      <c r="A49" s="40"/>
+      <c r="B49" s="43"/>
+      <c r="C49" s="43"/>
+      <c r="D49" s="43"/>
       <c r="E49" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="F49" s="26"/>
+        <v>75</v>
+      </c>
+      <c r="F49" s="38"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="43"/>
-      <c r="B50" s="46"/>
-      <c r="C50" s="46"/>
-      <c r="D50" s="46"/>
+      <c r="A50" s="41"/>
+      <c r="B50" s="44"/>
+      <c r="C50" s="44"/>
+      <c r="D50" s="44"/>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
     </row>
@@ -1510,16 +1523,16 @@
       <c r="F51" s="12"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="41">
+      <c r="A52" s="39">
         <v>11</v>
       </c>
-      <c r="B52" s="44" t="s">
+      <c r="B52" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="C52" s="44" t="s">
+      <c r="C52" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="D52" s="44" t="s">
+      <c r="D52" s="42" t="s">
         <v>33</v>
       </c>
       <c r="E52" s="24" t="s">
@@ -1528,20 +1541,20 @@
       <c r="F52" s="11"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" s="42"/>
-      <c r="B53" s="45"/>
-      <c r="C53" s="45"/>
-      <c r="D53" s="45"/>
+      <c r="A53" s="40"/>
+      <c r="B53" s="43"/>
+      <c r="C53" s="43"/>
+      <c r="D53" s="43"/>
       <c r="E53" s="24" t="s">
         <v>35</v>
       </c>
       <c r="F53" s="11"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="43"/>
-      <c r="B54" s="46"/>
-      <c r="C54" s="46"/>
-      <c r="D54" s="46"/>
+      <c r="A54" s="41"/>
+      <c r="B54" s="44"/>
+      <c r="C54" s="44"/>
+      <c r="D54" s="44"/>
       <c r="E54" s="24" t="s">
         <v>36</v>
       </c>
@@ -1555,16 +1568,16 @@
       <c r="E57" s="14"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A58" s="33">
+      <c r="A58" s="45">
         <v>6</v>
       </c>
-      <c r="B58" s="33" t="s">
+      <c r="B58" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C58" s="33" t="s">
+      <c r="C58" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="D58" s="33" t="s">
+      <c r="D58" s="45" t="s">
         <v>22</v>
       </c>
       <c r="E58" s="17" t="s">
@@ -1572,10 +1585,10 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A59" s="34"/>
-      <c r="B59" s="34"/>
-      <c r="C59" s="34"/>
-      <c r="D59" s="34"/>
+      <c r="A59" s="46"/>
+      <c r="B59" s="46"/>
+      <c r="C59" s="46"/>
+      <c r="D59" s="46"/>
       <c r="E59" s="17" t="s">
         <v>38</v>
       </c>
@@ -1601,7 +1614,7 @@
         <v>24</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
@@ -1610,7 +1623,7 @@
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
       <c r="E62" s="18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
@@ -1619,7 +1632,7 @@
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
       <c r="E63" s="18" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.35">
@@ -1656,10 +1669,6 @@
     <mergeCell ref="B52:B54"/>
     <mergeCell ref="C52:C54"/>
     <mergeCell ref="D52:D54"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="C48:C50"/>
-    <mergeCell ref="D48:D50"/>
     <mergeCell ref="A9:A17"/>
     <mergeCell ref="B9:B17"/>
     <mergeCell ref="C9:C17"/>
@@ -1672,11 +1681,11 @@
     <mergeCell ref="D30:D31"/>
     <mergeCell ref="B23:B25"/>
     <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
     <mergeCell ref="F48:F49"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="D48:D50"/>
     <mergeCell ref="D19:D21"/>
     <mergeCell ref="C19:C21"/>
     <mergeCell ref="B19:B21"/>
@@ -1689,6 +1698,10 @@
     <mergeCell ref="C33:C36"/>
     <mergeCell ref="D33:D36"/>
     <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>